<commit_message>
experiment build dict ok
</commit_message>
<xml_diff>
--- a/test/test_extractor/test_sheets/test_simple.xlsx
+++ b/test/test_extractor/test_sheets/test_simple.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oculardexterity/Documents/NUIM/LettersWork/processing-new/test/test-extractor/test-sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oculardexterity/Documents/NUIM/LettersWork/ProcessingNew/test/test_extractor/test_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>A_HEADER</t>
   </si>
@@ -39,12 +39,6 @@
   </si>
   <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>id_1</t>
-  </si>
-  <si>
-    <t>id_2</t>
   </si>
   <si>
     <t>a_value1</t>
@@ -427,7 +421,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -445,13 +439,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -461,8 +455,8 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
+      <c r="C3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>